<commit_message>
Messing up with the excel dissection data file
</commit_message>
<xml_diff>
--- a/adult-DSS-exp/exp1_DSS_dissection.xlsx
+++ b/adult-DSS-exp/exp1_DSS_dissection.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Chercheurs\Santos_Manuela\Thibault M\DSS\adult\dissection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Chercheurs\Santos_Manuela\Thibault M\gut-microbiota-iron\adult-DSS-exp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE44675-68C0-41AB-87B1-1DBFB63B0290}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC1B0E8-F3E4-40C2-8E8F-F884F57E0F70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{554E2A27-11F7-40A4-9E06-AA5D4B135DEF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
   <si>
     <t>Cage</t>
   </si>
@@ -188,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -211,11 +211,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -232,10 +252,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,7 +572,7 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,13 +604,13 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="8">
-        <v>50</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="9">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -611,9 +630,15 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
       <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
@@ -631,9 +656,15 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
       <c r="D4" s="5"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -641,11 +672,15 @@
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="A5" s="9">
         <v>3</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
+      <c r="B5" s="9">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
       <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
@@ -663,9 +698,15 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
+      <c r="A6" s="9">
+        <v>3</v>
+      </c>
+      <c r="B6" s="9">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
       <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
@@ -678,14 +719,20 @@
       <c r="G6" s="3">
         <v>0.10680000000000001</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="8">
         <v>1.5964</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
+      <c r="A7" s="9">
+        <v>3</v>
+      </c>
+      <c r="B7" s="9">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
       <c r="D7" s="5" t="s">
         <v>13</v>
       </c>
@@ -703,11 +750,15 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8" s="10">
         <v>5</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
+      <c r="B8" s="9">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
       <c r="D8" s="5" t="s">
         <v>14</v>
       </c>
@@ -725,9 +776,15 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
+      <c r="A9" s="10">
+        <v>5</v>
+      </c>
+      <c r="B9" s="9">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
       <c r="D9" s="5" t="s">
         <v>15</v>
       </c>
@@ -745,9 +802,15 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
+      <c r="A10" s="10">
+        <v>5</v>
+      </c>
+      <c r="B10" s="9">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
       <c r="D10" s="5" t="s">
         <v>16</v>
       </c>
@@ -765,13 +828,13 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="A11" s="10">
         <v>7</v>
       </c>
-      <c r="B11" s="8">
-        <v>500</v>
-      </c>
-      <c r="C11" s="8" t="s">
+      <c r="B11" s="9">
+        <v>500</v>
+      </c>
+      <c r="C11" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -791,9 +854,15 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
+      <c r="A12" s="10">
+        <v>7</v>
+      </c>
+      <c r="B12" s="9">
+        <v>500</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
       <c r="D12" s="5" t="s">
         <v>18</v>
       </c>
@@ -811,9 +880,15 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
+      <c r="A13" s="10">
+        <v>7</v>
+      </c>
+      <c r="B13" s="9">
+        <v>500</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
       <c r="D13" s="5" t="s">
         <v>19</v>
       </c>
@@ -831,11 +906,15 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="10">
         <v>9</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
+      <c r="B14" s="9">
+        <v>500</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
       <c r="D14" s="6" t="s">
         <v>20</v>
       </c>
@@ -853,9 +932,15 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
+      <c r="A15" s="10">
+        <v>9</v>
+      </c>
+      <c r="B15" s="9">
+        <v>500</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
       <c r="D15" s="6" t="s">
         <v>21</v>
       </c>
@@ -873,9 +958,15 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
+      <c r="A16" s="10">
+        <v>9</v>
+      </c>
+      <c r="B16" s="9">
+        <v>500</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
       <c r="D16" s="6" t="s">
         <v>22</v>
       </c>
@@ -893,11 +984,15 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
+      <c r="A17" s="10">
         <v>11</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
+      <c r="B17" s="9">
+        <v>500</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
       <c r="D17" s="6"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -905,9 +1000,15 @@
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
+      <c r="A18" s="10">
+        <v>11</v>
+      </c>
+      <c r="B18" s="9">
+        <v>500</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
       <c r="D18" s="6" t="s">
         <v>23</v>
       </c>
@@ -925,9 +1026,15 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
+      <c r="A19" s="10">
+        <v>11</v>
+      </c>
+      <c r="B19" s="9">
+        <v>500</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
       <c r="D19" s="6" t="s">
         <v>24</v>
       </c>
@@ -945,13 +1052,13 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
+      <c r="A20" s="10">
         <v>2</v>
       </c>
-      <c r="B20" s="8">
-        <v>50</v>
-      </c>
-      <c r="C20" s="8" t="s">
+      <c r="B20" s="10">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
         <v>25</v>
       </c>
       <c r="D20" s="7" t="s">
@@ -971,9 +1078,15 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
+      <c r="A21" s="10">
+        <v>2</v>
+      </c>
+      <c r="B21" s="10">
+        <v>50</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
       <c r="D21" s="7" t="s">
         <v>27</v>
       </c>
@@ -991,9 +1104,15 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
+      <c r="A22" s="10">
+        <v>2</v>
+      </c>
+      <c r="B22" s="10">
+        <v>50</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
       <c r="D22" s="7" t="s">
         <v>28</v>
       </c>
@@ -1011,11 +1130,15 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
+      <c r="A23" s="10">
         <v>4</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
+      <c r="B23" s="10">
+        <v>50</v>
+      </c>
+      <c r="C23" t="s">
+        <v>25</v>
+      </c>
       <c r="D23" s="7" t="s">
         <v>29</v>
       </c>
@@ -1033,9 +1156,15 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
+      <c r="A24" s="10">
+        <v>4</v>
+      </c>
+      <c r="B24" s="10">
+        <v>50</v>
+      </c>
+      <c r="C24" t="s">
+        <v>25</v>
+      </c>
       <c r="D24" s="7" t="s">
         <v>30</v>
       </c>
@@ -1053,9 +1182,15 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
+      <c r="A25" s="10">
+        <v>4</v>
+      </c>
+      <c r="B25" s="10">
+        <v>50</v>
+      </c>
+      <c r="C25" t="s">
+        <v>25</v>
+      </c>
       <c r="D25" s="7" t="s">
         <v>31</v>
       </c>
@@ -1073,11 +1208,15 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="8">
+      <c r="A26" s="10">
         <v>6</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
+      <c r="B26" s="10">
+        <v>50</v>
+      </c>
+      <c r="C26" t="s">
+        <v>25</v>
+      </c>
       <c r="D26" s="7" t="s">
         <v>32</v>
       </c>
@@ -1095,9 +1234,15 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
+      <c r="A27" s="10">
+        <v>6</v>
+      </c>
+      <c r="B27" s="10">
+        <v>50</v>
+      </c>
+      <c r="C27" t="s">
+        <v>25</v>
+      </c>
       <c r="D27" s="7" t="s">
         <v>33</v>
       </c>
@@ -1115,9 +1260,15 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
+      <c r="A28" s="10">
+        <v>6</v>
+      </c>
+      <c r="B28" s="10">
+        <v>50</v>
+      </c>
+      <c r="C28" t="s">
+        <v>25</v>
+      </c>
       <c r="D28" s="6"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -1125,13 +1276,13 @@
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="8">
-        <v>8</v>
-      </c>
-      <c r="B29" s="8">
-        <v>500</v>
-      </c>
-      <c r="C29" s="8" t="s">
+      <c r="A29" s="10">
+        <v>8</v>
+      </c>
+      <c r="B29" s="10">
+        <v>500</v>
+      </c>
+      <c r="C29" t="s">
         <v>25</v>
       </c>
       <c r="D29" s="7"/>
@@ -1141,9 +1292,15 @@
       <c r="H29" s="3"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
+      <c r="A30" s="10">
+        <v>8</v>
+      </c>
+      <c r="B30" s="10">
+        <v>500</v>
+      </c>
+      <c r="C30" t="s">
+        <v>25</v>
+      </c>
       <c r="D30" s="7" t="s">
         <v>34</v>
       </c>
@@ -1161,9 +1318,15 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
+      <c r="A31" s="10">
+        <v>8</v>
+      </c>
+      <c r="B31" s="10">
+        <v>500</v>
+      </c>
+      <c r="C31" t="s">
+        <v>25</v>
+      </c>
       <c r="D31" s="7" t="s">
         <v>35</v>
       </c>
@@ -1181,11 +1344,15 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="8">
+      <c r="A32" s="10">
         <v>10</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
+      <c r="B32" s="10">
+        <v>500</v>
+      </c>
+      <c r="C32" t="s">
+        <v>25</v>
+      </c>
       <c r="D32" s="7" t="s">
         <v>36</v>
       </c>
@@ -1203,9 +1370,15 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
+      <c r="A33" s="10">
+        <v>10</v>
+      </c>
+      <c r="B33" s="10">
+        <v>500</v>
+      </c>
+      <c r="C33" t="s">
+        <v>25</v>
+      </c>
       <c r="D33" s="7" t="s">
         <v>37</v>
       </c>
@@ -1223,9 +1396,15 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
+      <c r="A34" s="10">
+        <v>10</v>
+      </c>
+      <c r="B34" s="10">
+        <v>500</v>
+      </c>
+      <c r="C34" t="s">
+        <v>25</v>
+      </c>
       <c r="D34" s="7" t="s">
         <v>38</v>
       </c>
@@ -1243,11 +1422,15 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="8">
+      <c r="A35" s="10">
         <v>12</v>
       </c>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
+      <c r="B35" s="10">
+        <v>500</v>
+      </c>
+      <c r="C35" t="s">
+        <v>25</v>
+      </c>
       <c r="D35" s="7" t="s">
         <v>39</v>
       </c>
@@ -1265,9 +1448,15 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
+      <c r="A36" s="10">
+        <v>12</v>
+      </c>
+      <c r="B36" s="10">
+        <v>500</v>
+      </c>
+      <c r="C36" t="s">
+        <v>25</v>
+      </c>
       <c r="D36" s="7" t="s">
         <v>40</v>
       </c>
@@ -1285,9 +1474,15 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
+      <c r="A37" s="10">
+        <v>12</v>
+      </c>
+      <c r="B37" s="10">
+        <v>500</v>
+      </c>
+      <c r="C37" t="s">
+        <v>25</v>
+      </c>
       <c r="D37" s="7" t="s">
         <v>41</v>
       </c>
@@ -1305,28 +1500,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B19"/>
-    <mergeCell ref="C11:C19"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B10"/>
-    <mergeCell ref="C2:C10"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B37"/>
-    <mergeCell ref="C29:C37"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B28"/>
-    <mergeCell ref="C20:C28"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A26:A28"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding age at start of exp into excel dissec file
</commit_message>
<xml_diff>
--- a/adult-DSS-exp/exp1_DSS_dissection.xlsx
+++ b/adult-DSS-exp/exp1_DSS_dissection.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Chercheurs\Santos_Manuela\Thibault M\gut-microbiota-iron\adult-DSS-exp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CHUM_git\gut-microbiota-iron\adult-DSS-exp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC1B0E8-F3E4-40C2-8E8F-F884F57E0F70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55096CE8-09C2-4A4D-B5BE-238464734D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{554E2A27-11F7-40A4-9E06-AA5D4B135DEF}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{554E2A27-11F7-40A4-9E06-AA5D4B135DEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="44">
   <si>
     <t>Cage</t>
   </si>
@@ -151,6 +162,12 @@
   </si>
   <si>
     <t>15912B</t>
+  </si>
+  <si>
+    <t>Pedigree prefix</t>
+  </si>
+  <si>
+    <t>Age start (d)</t>
   </si>
 </sst>
 </file>
@@ -235,26 +252,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -273,9 +288,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -313,7 +328,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -419,7 +434,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -561,7 +576,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -569,15 +584,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00701608-0F56-4BE8-8AA0-3F6DA00B883D}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -602,12 +617,18 @@
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+      <c r="I1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="7">
         <v>50</v>
       </c>
       <c r="C2" t="s">
@@ -628,12 +649,18 @@
       <c r="H2" s="3">
         <v>1.2230000000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="7">
         <v>50</v>
       </c>
       <c r="C3" t="s">
@@ -654,12 +681,18 @@
       <c r="H3" s="3">
         <v>1.5378000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="7">
         <v>50</v>
       </c>
       <c r="C4" t="s">
@@ -671,11 +704,11 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A5" s="7">
         <v>3</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="7">
         <v>50</v>
       </c>
       <c r="C5" t="s">
@@ -696,12 +729,18 @@
       <c r="H5" s="3">
         <v>1.0091000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A6" s="7">
         <v>3</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="7">
         <v>50</v>
       </c>
       <c r="C6" t="s">
@@ -719,15 +758,21 @@
       <c r="G6" s="3">
         <v>0.10680000000000001</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="3">
         <v>1.5964</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="I6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A7" s="7">
         <v>3</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="7">
         <v>50</v>
       </c>
       <c r="C7" t="s">
@@ -748,12 +793,18 @@
       <c r="H7" s="3">
         <v>1.3727</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+      <c r="I7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A8" s="8">
         <v>5</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="7">
         <v>50</v>
       </c>
       <c r="C8" t="s">
@@ -774,12 +825,18 @@
       <c r="H8" s="3">
         <v>1.3036000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A9" s="8">
         <v>5</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="7">
         <v>50</v>
       </c>
       <c r="C9" t="s">
@@ -800,12 +857,18 @@
       <c r="H9" s="3">
         <v>1.0355000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+      <c r="I9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A10" s="8">
         <v>5</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="7">
         <v>50</v>
       </c>
       <c r="C10" t="s">
@@ -826,12 +889,18 @@
       <c r="H10" s="3">
         <v>1.0784</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
+      <c r="I10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A11" s="8">
         <v>7</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="7">
         <v>500</v>
       </c>
       <c r="C11" t="s">
@@ -852,12 +921,18 @@
       <c r="H11" s="3">
         <v>0.83679999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
+      <c r="I11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A12" s="8">
         <v>7</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="7">
         <v>500</v>
       </c>
       <c r="C12" t="s">
@@ -878,12 +953,18 @@
       <c r="H12" s="3">
         <v>1.155</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
+      <c r="I12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A13" s="8">
         <v>7</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="7">
         <v>500</v>
       </c>
       <c r="C13" t="s">
@@ -904,18 +985,24 @@
       <c r="H13" s="3">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
+      <c r="I13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A14" s="8">
         <v>9</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="7">
         <v>500</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E14" s="3">
@@ -930,18 +1017,24 @@
       <c r="H14" s="3">
         <v>1.536</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
+      <c r="I14" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A15" s="8">
         <v>9</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="7">
         <v>500</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E15" s="3">
@@ -956,18 +1049,24 @@
       <c r="H15" s="3">
         <v>1.4283999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
+      <c r="I15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A16" s="8">
         <v>9</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="7">
         <v>500</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E16" s="3">
@@ -982,34 +1081,40 @@
       <c r="H16" s="3">
         <v>1.3418000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
+      <c r="I16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A17" s="8">
         <v>11</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="7">
         <v>500</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="6"/>
+      <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A18" s="8">
         <v>11</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="7">
         <v>500</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E18" s="3">
@@ -1024,18 +1129,24 @@
       <c r="H18" s="3">
         <v>1.2943</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
+      <c r="I18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J18">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A19" s="8">
         <v>11</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="7">
         <v>500</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E19" s="3">
@@ -1050,18 +1161,24 @@
       <c r="H19" s="3">
         <v>1.6427</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
+      <c r="I19" t="s">
+        <v>24</v>
+      </c>
+      <c r="J19">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A20" s="8">
         <v>2</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="8">
         <v>50</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>26</v>
       </c>
       <c r="E20" s="3">
@@ -1076,18 +1193,24 @@
       <c r="H20" s="3">
         <v>1.4539</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
+      <c r="I20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J20">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A21" s="8">
         <v>2</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="8">
         <v>50</v>
       </c>
       <c r="C21" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="6" t="s">
         <v>27</v>
       </c>
       <c r="E21" s="3">
@@ -1102,18 +1225,24 @@
       <c r="H21" s="3">
         <v>1.2562</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="10">
+      <c r="I21" t="s">
+        <v>27</v>
+      </c>
+      <c r="J21">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A22" s="8">
         <v>2</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="8">
         <v>50</v>
       </c>
       <c r="C22" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E22" s="3">
@@ -1128,18 +1257,24 @@
       <c r="H22" s="3">
         <v>0.98740000000000006</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="10">
+      <c r="I22" t="s">
+        <v>28</v>
+      </c>
+      <c r="J22">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A23" s="8">
         <v>4</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23" s="8">
         <v>50</v>
       </c>
       <c r="C23" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E23" s="3">
@@ -1154,18 +1289,24 @@
       <c r="H23" s="3">
         <v>0.71240000000000003</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
+      <c r="I23" t="s">
+        <v>29</v>
+      </c>
+      <c r="J23">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A24" s="8">
         <v>4</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B24" s="8">
         <v>50</v>
       </c>
       <c r="C24" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E24" s="3">
@@ -1180,18 +1321,24 @@
       <c r="H24" s="3">
         <v>1.1854</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="10">
+      <c r="I24" t="s">
+        <v>30</v>
+      </c>
+      <c r="J24">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A25" s="8">
         <v>4</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="8">
         <v>50</v>
       </c>
       <c r="C25" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="6" t="s">
         <v>31</v>
       </c>
       <c r="E25" s="3">
@@ -1206,18 +1353,24 @@
       <c r="H25" s="3">
         <v>1.1125</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="10">
+      <c r="I25" t="s">
+        <v>31</v>
+      </c>
+      <c r="J25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A26" s="8">
         <v>6</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B26" s="8">
         <v>50</v>
       </c>
       <c r="C26" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="6" t="s">
         <v>32</v>
       </c>
       <c r="E26" s="3">
@@ -1232,18 +1385,24 @@
       <c r="H26" s="3">
         <v>1.1559999999999999</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="10">
+      <c r="I26" t="s">
+        <v>32</v>
+      </c>
+      <c r="J26">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A27" s="8">
         <v>6</v>
       </c>
-      <c r="B27" s="10">
+      <c r="B27" s="8">
         <v>50</v>
       </c>
       <c r="C27" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="6" t="s">
         <v>33</v>
       </c>
       <c r="E27" s="3">
@@ -1258,50 +1417,56 @@
       <c r="H27" s="3">
         <v>1.2605</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="10">
+      <c r="I27" t="s">
+        <v>33</v>
+      </c>
+      <c r="J27">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A28" s="8">
         <v>6</v>
       </c>
-      <c r="B28" s="10">
+      <c r="B28" s="8">
         <v>50</v>
       </c>
       <c r="C28" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="6"/>
+      <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="10">
-        <v>8</v>
-      </c>
-      <c r="B29" s="10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A29" s="8">
+        <v>8</v>
+      </c>
+      <c r="B29" s="8">
         <v>500</v>
       </c>
       <c r="C29" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="7"/>
+      <c r="D29" s="6"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="10">
-        <v>8</v>
-      </c>
-      <c r="B30" s="10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A30" s="8">
+        <v>8</v>
+      </c>
+      <c r="B30" s="8">
         <v>500</v>
       </c>
       <c r="C30" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E30" s="3">
@@ -1316,18 +1481,24 @@
       <c r="H30" s="3">
         <v>1.4784999999999999</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="10">
-        <v>8</v>
-      </c>
-      <c r="B31" s="10">
+      <c r="I30" t="s">
+        <v>34</v>
+      </c>
+      <c r="J30">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A31" s="8">
+        <v>8</v>
+      </c>
+      <c r="B31" s="8">
         <v>500</v>
       </c>
       <c r="C31" t="s">
         <v>25</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="6" t="s">
         <v>35</v>
       </c>
       <c r="E31" s="3">
@@ -1342,18 +1513,24 @@
       <c r="H31" s="3">
         <v>1.4522999999999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="10">
+      <c r="I31" t="s">
+        <v>35</v>
+      </c>
+      <c r="J31">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A32" s="8">
         <v>10</v>
       </c>
-      <c r="B32" s="10">
+      <c r="B32" s="8">
         <v>500</v>
       </c>
       <c r="C32" t="s">
         <v>25</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="6" t="s">
         <v>36</v>
       </c>
       <c r="E32" s="3">
@@ -1368,18 +1545,24 @@
       <c r="H32" s="3">
         <v>1.0336000000000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="10">
+      <c r="I32" t="s">
+        <v>36</v>
+      </c>
+      <c r="J32">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A33" s="8">
         <v>10</v>
       </c>
-      <c r="B33" s="10">
+      <c r="B33" s="8">
         <v>500</v>
       </c>
       <c r="C33" t="s">
         <v>25</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="6" t="s">
         <v>37</v>
       </c>
       <c r="E33" s="3">
@@ -1394,18 +1577,24 @@
       <c r="H33" s="3">
         <v>1.1023000000000001</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="10">
+      <c r="I33" t="s">
+        <v>37</v>
+      </c>
+      <c r="J33">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A34" s="8">
         <v>10</v>
       </c>
-      <c r="B34" s="10">
+      <c r="B34" s="8">
         <v>500</v>
       </c>
       <c r="C34" t="s">
         <v>25</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="6" t="s">
         <v>38</v>
       </c>
       <c r="E34" s="3">
@@ -1420,18 +1609,24 @@
       <c r="H34" s="3">
         <v>0.95889999999999997</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="10">
+      <c r="I34" t="s">
+        <v>38</v>
+      </c>
+      <c r="J34">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A35" s="8">
         <v>12</v>
       </c>
-      <c r="B35" s="10">
+      <c r="B35" s="8">
         <v>500</v>
       </c>
       <c r="C35" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="6" t="s">
         <v>39</v>
       </c>
       <c r="E35" s="3">
@@ -1446,18 +1641,24 @@
       <c r="H35" s="3">
         <v>1.4414</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="10">
+      <c r="I35" t="s">
+        <v>39</v>
+      </c>
+      <c r="J35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A36" s="8">
         <v>12</v>
       </c>
-      <c r="B36" s="10">
+      <c r="B36" s="8">
         <v>500</v>
       </c>
       <c r="C36" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="6" t="s">
         <v>40</v>
       </c>
       <c r="E36" s="3">
@@ -1472,18 +1673,24 @@
       <c r="H36" s="3">
         <v>1.1716</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="10">
+      <c r="I36" t="s">
+        <v>40</v>
+      </c>
+      <c r="J36">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A37" s="8">
         <v>12</v>
       </c>
-      <c r="B37" s="10">
+      <c r="B37" s="8">
         <v>500</v>
       </c>
       <c r="C37" t="s">
         <v>25</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="6" t="s">
         <v>41</v>
       </c>
       <c r="E37" s="3">
@@ -1497,6 +1704,12 @@
       </c>
       <c r="H37" s="3">
         <v>1.2604</v>
+      </c>
+      <c r="I37" t="s">
+        <v>41</v>
+      </c>
+      <c r="J37">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>